<commit_message>
updated doc- sprint 1
</commit_message>
<xml_diff>
--- a/Deskify Documents/Product-Backlog.xlsx
+++ b/Deskify Documents/Product-Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwetha.b\Desktop\Documents\New-Deskify\Deskify Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwetha.b\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7555D5-39A1-449F-9EDF-D7FFE918A7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AD88D54-A11F-4DCD-A881-28325C1D0D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="112">
   <si>
     <t>#</t>
   </si>
@@ -121,12 +121,6 @@
     <t>Story point estimation</t>
   </si>
   <si>
-    <t>Registration and Login</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
     <t>REQ4</t>
   </si>
   <si>
@@ -151,48 +145,18 @@
     <t>Prompt Questionnaries</t>
   </si>
   <si>
-    <t>Registration for new user</t>
-  </si>
-  <si>
-    <t>Login page for registered user</t>
-  </si>
-  <si>
-    <t>Logout from application</t>
-  </si>
-  <si>
-    <t>UI functionality for profile</t>
-  </si>
-  <si>
     <t>Test case preparation and Unit Testing</t>
   </si>
   <si>
-    <t>Book Seat</t>
-  </si>
-  <si>
     <t>View Pass</t>
   </si>
   <si>
-    <t>View Booking</t>
-  </si>
-  <si>
     <t>Modify Booking</t>
   </si>
   <si>
     <t>Cancel Booking</t>
   </si>
   <si>
-    <t>UI functionality for dashboard</t>
-  </si>
-  <si>
-    <t>View Profile</t>
-  </si>
-  <si>
-    <t>Modify Profile</t>
-  </si>
-  <si>
-    <t>UI functionality for Profile</t>
-  </si>
-  <si>
     <t>Notification for Booked Seat</t>
   </si>
   <si>
@@ -229,9 +193,6 @@
     <t>UI functionality for Prompt Questinnaries</t>
   </si>
   <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
     <t>Add/Delete Room</t>
   </si>
   <si>
@@ -241,17 +202,185 @@
     <t>Add/Delete Seat</t>
   </si>
   <si>
-    <t>In-Progress</t>
-  </si>
-  <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Database Schema</t>
+  </si>
+  <si>
+    <t>Creative Models</t>
+  </si>
+  <si>
+    <t>Integrating with My SQL Server</t>
+  </si>
+  <si>
+    <t>Database generation</t>
+  </si>
+  <si>
+    <t>Adding and implementing classes for Registartion</t>
+  </si>
+  <si>
+    <t>Adding Business layer for registartion</t>
+  </si>
+  <si>
+    <t>Creating Controller API</t>
+  </si>
+  <si>
+    <t>MVC for registration</t>
+  </si>
+  <si>
+    <t>UI design for registration</t>
+  </si>
+  <si>
+    <t>UI design for header</t>
+  </si>
+  <si>
+    <t>Test cases for Registration</t>
+  </si>
+  <si>
+    <t>New User Registration</t>
+  </si>
+  <si>
+    <t>Login and Logout</t>
+  </si>
+  <si>
+    <t>Adding and implementing classes for Login and Logout</t>
+  </si>
+  <si>
+    <t>Adding Business layer for  Login and Logout</t>
+  </si>
+  <si>
+    <t>MVC for Login and Logout</t>
+  </si>
+  <si>
+    <t>Rediecting Logic</t>
+  </si>
+  <si>
+    <t>UI for Login and Logout</t>
+  </si>
+  <si>
+    <t>Test cases for Login and logout</t>
+  </si>
+  <si>
+    <t>Forgot Password</t>
+  </si>
+  <si>
+    <t>Adding Logic in API</t>
+  </si>
+  <si>
+    <t>Creating MVC</t>
+  </si>
+  <si>
+    <t>UI design for Forgot Password</t>
+  </si>
+  <si>
+    <t>Test cases for Forgot Password</t>
+  </si>
+  <si>
+    <t>User Dashboard</t>
+  </si>
+  <si>
+    <t>Adding and implementing classes</t>
+  </si>
+  <si>
+    <t>Adding Business layer for  Booking seat</t>
+  </si>
+  <si>
+    <t>MVC for Booking seat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UI for view seat/meeting pass</t>
+  </si>
+  <si>
+    <t>UI for seat Booking</t>
+  </si>
+  <si>
+    <t>UI for Status card</t>
+  </si>
+  <si>
+    <t>UI for redirecting  to notification, profile and logout</t>
+  </si>
+  <si>
+    <t>Adding Booking seat test cases</t>
+  </si>
+  <si>
+    <t>Modify Booking seat test cases</t>
+  </si>
+  <si>
+    <t>Cancel Booking seat test cases</t>
+  </si>
+  <si>
+    <t>Get all Booking seat test cases</t>
+  </si>
+  <si>
+    <t>Test cases for Seat Booking</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>Adding Interface for employee</t>
+  </si>
+  <si>
+    <t>Implemnting classes for employee</t>
+  </si>
+  <si>
+    <t>Adding Business layer for employee</t>
+  </si>
+  <si>
+    <t>Creating API Controller</t>
+  </si>
+  <si>
+    <t>MVC for Employee Controller</t>
+  </si>
+  <si>
+    <t>Test cases for Add employee</t>
+  </si>
+  <si>
+    <t>Test cases for Modify employee</t>
+  </si>
+  <si>
+    <t>Test cases for Delete employee</t>
+  </si>
+  <si>
+    <t>Test cases for get all employee</t>
+  </si>
+  <si>
+    <t>UI design for profile</t>
+  </si>
+  <si>
+    <t>REQ8</t>
+  </si>
+  <si>
+    <t>REQ08 - Continous Integration</t>
+  </si>
+  <si>
+    <t>CI/CD Pipeline and Azure app service</t>
+  </si>
+  <si>
+    <t>Boards in azure devops</t>
+  </si>
+  <si>
+    <t>REQ9</t>
+  </si>
+  <si>
+    <t>REQ10</t>
+  </si>
+  <si>
+    <t>REQ11</t>
+  </si>
+  <si>
+    <t>REQ12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +423,23 @@
     <font>
       <b/>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -394,10 +540,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -457,11 +604,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4 2 2" xfId="1" xr:uid="{82F39933-7FBD-4D62-80A5-FD4166B1C4C7}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
     <dxf>
       <font>
         <strike val="0"/>
@@ -469,6 +627,82 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -574,10 +808,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>343</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -620,7 +854,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>343</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1308,13 +1542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,7 +1559,8 @@
     <col min="4" max="4" width="43.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="5.21875" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.21875" style="1" customWidth="1"/>
@@ -1424,11 +1659,11 @@
       <c r="G5" s="2"/>
       <c r="H5" s="5">
         <f>SUM(H6:H24)</f>
-        <v>343</v>
+        <v>59</v>
       </c>
       <c r="I5" s="5">
         <f>SUM(I6:I24)</f>
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="J5" s="5">
         <f>SUM(J6:J24)</f>
@@ -1458,8 +1693,8 @@
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>27</v>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1475,7 +1710,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>19</v>
@@ -1484,13 +1719,13 @@
         <v>24</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H8" s="15">
-        <v>28</v>
-      </c>
-      <c r="I8" s="3">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="I8" s="20">
+        <v>3</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1500,7 +1735,7 @@
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>19</v>
@@ -1509,13 +1744,13 @@
         <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H9" s="15">
-        <v>20</v>
-      </c>
-      <c r="I9" s="3">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="I9" s="20">
+        <v>3</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1525,7 +1760,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>19</v>
@@ -1534,12 +1769,12 @@
         <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H10" s="15">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="20">
         <v>7</v>
       </c>
       <c r="J10" s="3"/>
@@ -1550,7 +1785,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>19</v>
@@ -1559,13 +1794,13 @@
         <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H11" s="15">
-        <v>25</v>
-      </c>
-      <c r="I11" s="3">
-        <v>25</v>
+        <v>3</v>
+      </c>
+      <c r="I11" s="20">
+        <v>1</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1574,19 +1809,11 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="15">
-        <v>34</v>
-      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1612,16 +1839,26 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="G14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="15">
+        <v>3</v>
+      </c>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
@@ -1629,20 +1866,22 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="14" t="s">
-        <v>42</v>
+      <c r="D15" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H15" s="15">
-        <v>25</v>
-      </c>
-      <c r="I15" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I15" s="20">
+        <v>1</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
@@ -1651,19 +1890,21 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="H16" s="15">
-        <v>40</v>
-      </c>
-      <c r="I16" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I16" s="20">
+        <v>2</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
@@ -1672,19 +1913,21 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H17" s="15">
-        <v>15</v>
-      </c>
-      <c r="I17" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I17" s="20">
+        <v>2</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -1693,19 +1936,21 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H18" s="15">
-        <v>20</v>
-      </c>
-      <c r="I18" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="I18" s="20">
+        <v>5</v>
+      </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
@@ -1713,20 +1958,22 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="14" t="s">
-        <v>46</v>
+      <c r="D19" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H19" s="15">
-        <v>20</v>
-      </c>
-      <c r="I19" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="I19" s="20">
+        <v>4</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
@@ -1734,20 +1981,22 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="14" t="s">
-        <v>47</v>
+      <c r="D20" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H20" s="15">
-        <v>44</v>
-      </c>
-      <c r="I20" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="I20" s="20">
+        <v>3</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
@@ -1755,19 +2004,11 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="15">
-        <v>40</v>
-      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1785,7 +2026,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>3</v>
       </c>
@@ -1793,16 +2034,26 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="G23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="15">
+        <v>4</v>
+      </c>
+      <c r="I23" s="20">
+        <v>2</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
@@ -1811,19 +2062,21 @@
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H24" s="15">
-        <v>25</v>
-      </c>
-      <c r="I24" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I24" s="20">
+        <v>1</v>
+      </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
@@ -1832,19 +2085,21 @@
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H25" s="15">
-        <v>20</v>
-      </c>
-      <c r="I25" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I25" s="20">
+        <v>2</v>
+      </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
@@ -1853,19 +2108,21 @@
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="H26" s="15">
-        <v>22</v>
-      </c>
-      <c r="I26" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I26" s="20">
+        <v>3</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
@@ -1874,525 +2131,1378 @@
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="H27" s="15">
-        <v>30</v>
-      </c>
-      <c r="I27" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="I27" s="20">
+        <v>2</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="15">
+        <v>6</v>
+      </c>
+      <c r="I28" s="21">
+        <v>4</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="E29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="15">
+        <v>3</v>
+      </c>
+      <c r="I29" s="20">
+        <v>3</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="A31" s="3">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="D31" s="4" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H31" s="15">
+        <v>4</v>
+      </c>
+      <c r="I31" s="20">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="H32" s="15">
+        <v>3</v>
+      </c>
+      <c r="I32" s="20">
+        <v>3</v>
+      </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="15">
+        <v>4</v>
+      </c>
+      <c r="I33" s="21">
+        <v>3</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
-        <v>5</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="15">
+        <v>2</v>
+      </c>
+      <c r="I34" s="20">
+        <v>2</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="A36" s="3">
+        <v>5</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="D36" s="4" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H36" s="15">
+        <v>4</v>
+      </c>
+      <c r="I36" s="20">
+        <v>2</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H37" s="15">
+        <v>3</v>
+      </c>
+      <c r="I37" s="20">
+        <v>2</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H38" s="15">
+        <v>3</v>
+      </c>
+      <c r="I38" s="20">
+        <v>2</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="3"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="15">
+        <v>5</v>
+      </c>
+      <c r="I39" s="20">
+        <v>4</v>
+      </c>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="15">
         <v>6</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="I40" s="20">
+        <v>8</v>
+      </c>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H41" s="15">
+        <v>3</v>
+      </c>
+      <c r="I41" s="20">
+        <v>3</v>
+      </c>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H42" s="15">
+        <v>3</v>
+      </c>
+      <c r="I42" s="20">
+        <v>3</v>
+      </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H43" s="15">
+        <v>8</v>
+      </c>
+      <c r="I43" s="21">
+        <v>8</v>
+      </c>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H44" s="15">
+        <v>8</v>
+      </c>
+      <c r="I44" s="21">
+        <v>7</v>
+      </c>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="H45" s="15">
+        <v>5</v>
+      </c>
+      <c r="I45" s="21">
+        <v>2</v>
+      </c>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H46" s="15">
+        <v>6</v>
+      </c>
+      <c r="I46" s="21">
+        <v>4</v>
+      </c>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="G47" s="4"/>
       <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="A48" s="4">
+        <v>6</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="D48" s="4" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H48" s="15">
+        <v>1</v>
+      </c>
+      <c r="I48" s="20">
+        <v>2</v>
+      </c>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="B49" s="3"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H49" s="15">
+        <v>1</v>
+      </c>
+      <c r="I49" s="20">
+        <v>2</v>
+      </c>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="B50" s="3"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
+      <c r="D50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H50" s="15">
+        <v>1</v>
+      </c>
+      <c r="I50" s="20">
+        <v>1</v>
+      </c>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="3">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" s="15">
+        <v>1</v>
+      </c>
+      <c r="I51" s="20">
+        <v>2</v>
+      </c>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
         <v>7</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
+      <c r="B53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="D53" s="4" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H53" s="15">
+        <v>2</v>
+      </c>
+      <c r="I53" s="20">
+        <v>3</v>
+      </c>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="B54" s="3"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="H54" s="15">
+        <v>2</v>
+      </c>
+      <c r="I54" s="20">
+        <v>2</v>
+      </c>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="B55" s="3"/>
       <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
+      <c r="D55" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
+      <c r="G55" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H55" s="15">
+        <v>1</v>
+      </c>
+      <c r="I55" s="20">
+        <v>2</v>
+      </c>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56" s="15">
+        <v>3</v>
+      </c>
+      <c r="I56" s="20">
+        <v>2</v>
+      </c>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H57" s="15">
+        <v>4</v>
+      </c>
+      <c r="I57" s="20">
+        <v>2</v>
+      </c>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="4"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H58" s="15">
+        <v>1</v>
+      </c>
+      <c r="I58" s="20">
+        <v>2</v>
+      </c>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H59" s="15">
+        <v>1</v>
+      </c>
+      <c r="I59" s="20">
+        <v>3</v>
+      </c>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H60" s="15">
+        <v>1</v>
+      </c>
+      <c r="I60" s="20">
+        <v>2</v>
+      </c>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H61" s="15">
+        <v>1</v>
+      </c>
+      <c r="I61" s="20">
+        <v>3</v>
+      </c>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H62" s="15">
+        <v>5</v>
+      </c>
+      <c r="I62" s="20">
+        <v>3</v>
+      </c>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
+        <v>8</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H64" s="15">
+        <v>6</v>
+      </c>
+      <c r="I64" s="20">
+        <v>7</v>
+      </c>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H65" s="15">
+        <v>8</v>
+      </c>
+      <c r="I65" s="23">
+        <v>7</v>
+      </c>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>9</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="4"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <v>10</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>11</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>12</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2400,25 +3510,83 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A6:D6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G6:G21 G23:G54">
-    <cfRule type="cellIs" dxfId="4" priority="37" operator="equal">
+  <conditionalFormatting sqref="G6:G11 G13:G20 G23:G92">
+    <cfRule type="cellIs" dxfId="14" priority="67" operator="equal">
       <formula>"In-Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="68" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G21 G23:G54">
-    <cfRule type="cellIs" dxfId="2" priority="174" operator="equal">
+  <conditionalFormatting sqref="H30">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"In-Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="176" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+      <formula>"In-Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="177">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"In-Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"In-Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Not Started"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G11 G13:G20 G23:G92">
+    <cfRule type="cellIs" dxfId="2" priority="212" operator="equal">
+      <formula>"In-Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="213" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="214" operator="equal">
+      <formula>"Not Started"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="215">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2430,10 +3598,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G21 G23:G54" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G20 G23:G92" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Not Started,In-Progress,Completed,Removed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:F27 F7:F21" xr:uid="{5EB879C5-3EBD-4A6A-BA72-330D8D9C819B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:F66 F7:F21" xr:uid="{5EB879C5-3EBD-4A6A-BA72-330D8D9C819B}">
       <formula1>"P1,P2,P3"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2446,7 +3614,7 @@
           <x14:formula1>
             <xm:f>'Release Phase'!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:E21 E23:E27 E29:E32 E35:E38 E41:E49 E52:E54</xm:sqref>
+          <xm:sqref>E90:E92 G21:H21 E67:E70 E73:E76 E79:E87 E8:E21 E23:E66</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2458,7 +3626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -2484,7 +3652,7 @@
       </c>
       <c r="C3">
         <f>'Product Backlog'!H5</f>
-        <v>343</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>